<commit_message>
interm commit working towards multiple data files
</commit_message>
<xml_diff>
--- a/plotly-dash/data/pyqt-dash-config.xlsx
+++ b/plotly-dash/data/pyqt-dash-config.xlsx
@@ -16,6 +16,8 @@
     <sheet name="graph01" sheetId="2" r:id="rId2"/>
     <sheet name="graph02" sheetId="3" r:id="rId3"/>
     <sheet name="graph03" sheetId="4" r:id="rId4"/>
+    <sheet name="graph04" sheetId="5" r:id="rId5"/>
+    <sheet name="graph05" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="56">
   <si>
     <t>Dash Experiments</t>
   </si>
@@ -61,9 +63,6 @@
     <t>Height</t>
   </si>
   <si>
-    <t>Position</t>
-  </si>
-  <si>
     <t>xValue</t>
   </si>
   <si>
@@ -138,6 +137,78 @@
   <si>
     <t>This is a MarkDown header.    
 Attempting to use *Dash* for plotting in PyQt5.</t>
+  </si>
+  <si>
+    <t>Datafile</t>
+  </si>
+  <si>
+    <t>data/tp05j2a.rgeo</t>
+  </si>
+  <si>
+    <t>Missile position</t>
+  </si>
+  <si>
+    <t>position.w[0]</t>
+  </si>
+  <si>
+    <t>position.w[1]</t>
+  </si>
+  <si>
+    <t>position.w[2]</t>
+  </si>
+  <si>
+    <t>data/tp05j2a_Observer0.traj</t>
+  </si>
+  <si>
+    <t>Relative position</t>
+  </si>
+  <si>
+    <t>Relative speed</t>
+  </si>
+  <si>
+    <t>data/tp05j2a_Observer0.gmbl</t>
+  </si>
+  <si>
+    <t>%t</t>
+  </si>
+  <si>
+    <t>gimbrol</t>
+  </si>
+  <si>
+    <t>gimbpit</t>
+  </si>
+  <si>
+    <t>gimbyaw</t>
+  </si>
+  <si>
+    <t>Gimbal rol</t>
+  </si>
+  <si>
+    <t>Gimbal pitch</t>
+  </si>
+  <si>
+    <t>Gimbal yaw</t>
+  </si>
+  <si>
+    <t>rol</t>
+  </si>
+  <si>
+    <t>pit</t>
+  </si>
+  <si>
+    <t>yaw</t>
+  </si>
+  <si>
+    <t>Missile pitch</t>
+  </si>
+  <si>
+    <t>Missile yaw</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Missile rol/100</t>
   </si>
 </sst>
 </file>
@@ -521,7 +592,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -532,10 +603,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +615,7 @@
     <col min="2" max="2" width="40" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -552,93 +623,119 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -648,10 +745,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +757,7 @@
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -668,93 +765,119 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -764,10 +887,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,7 +899,7 @@
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -784,51 +907,369 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
       <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
various updates for default settings
</commit_message>
<xml_diff>
--- a/plotly-dash/data/pyqt-dash-config.xlsx
+++ b/plotly-dash/data/pyqt-dash-config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22305" windowHeight="11610" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22305" windowHeight="11610" tabRatio="686" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="header" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="graph03" sheetId="4" r:id="rId4"/>
     <sheet name="graph04" sheetId="5" r:id="rId5"/>
     <sheet name="graph05" sheetId="6" r:id="rId6"/>
+    <sheet name="documentation" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="88">
   <si>
     <t>Dash Experiments</t>
   </si>
@@ -72,9 +73,6 @@
     <t>yValue</t>
   </si>
   <si>
-    <t>LineType</t>
-  </si>
-  <si>
     <t>%CurrentSimTime</t>
   </si>
   <si>
@@ -90,9 +88,6 @@
     <t>Rel-loc-World[2]</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Distance</t>
   </si>
   <si>
@@ -100,9 +95,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>Time</t>
   </si>
   <si>
     <t>Z</t>
@@ -224,13 +216,103 @@
   </si>
   <si>
     <t>Distance [m]</t>
+  </si>
+  <si>
+    <t>Velocity [m/s]</t>
+  </si>
+  <si>
+    <t>Attitude [rad]</t>
+  </si>
+  <si>
+    <t>Relative x [m]</t>
+  </si>
+  <si>
+    <t>Relative y [m]</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Dash</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>Linewidth</t>
+  </si>
+  <si>
+    <t>Linewidth is the line width in pt</t>
+  </si>
+  <si>
+    <t>rgb(67,67,67)</t>
+  </si>
+  <si>
+    <t>color can have many different formats</t>
+  </si>
+  <si>
+    <t>rgba(0,100,80,0.2)</t>
+  </si>
+  <si>
+    <t>https://community.plot.ly/t/plotly-colours-list/11730/3</t>
+  </si>
+  <si>
+    <t>cyan</t>
+  </si>
+  <si>
+    <t>goldenrod</t>
+  </si>
+  <si>
+    <t>palegreen</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/cssref/css_colors.asp</t>
+  </si>
+  <si>
+    <t>https://www.rapidtables.com/web/css/css-color.html</t>
+  </si>
+  <si>
+    <t>dot</t>
+  </si>
+  <si>
+    <t>dash</t>
+  </si>
+  <si>
+    <t>dashdot</t>
+  </si>
+  <si>
+    <t>dash options include 'dash', 'dot', and 'dashdot' or leave empty for normal line</t>
+  </si>
+  <si>
+    <t>BlueViolet</t>
+  </si>
+  <si>
+    <t>GraphType</t>
+  </si>
+  <si>
+    <t>LineLabel</t>
+  </si>
+  <si>
+    <t>can be 'line' (default) or 'bar', I am nit sure what this really helps.</t>
+  </si>
+  <si>
+    <t>default if not given is 'line'</t>
+  </si>
+  <si>
+    <t>by default plotly will assign its own colours if not supplied.</t>
+  </si>
+  <si>
+    <t>Default if not given, use solid line</t>
+  </si>
+  <si>
+    <t>Default if not given, use plotly default</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,10 +333,18 @@
       <family val="3"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF448C27"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -274,28 +364,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -606,8 +700,8 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>31</v>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -618,151 +712,193 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" style="3" customWidth="1"/>
     <col min="2" max="2" width="40" style="4" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="3"/>
+    <col min="6" max="6" width="12.42578125" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="3">
+        <v>4</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="4">
@@ -770,16 +906,19 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F7" r:id="rId1" display="https://www.w3schools.com/colors/color_tryit.asp?color=BlueViolet"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,7 +927,7 @@
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -796,130 +935,136 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -934,10 +1079,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,7 +1091,7 @@
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -954,79 +1099,91 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1041,10 +1198,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="D7" sqref="D7:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1210,7 @@
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1061,113 +1218,110 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
+      <c r="B6" t="s">
+        <v>10</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>35</v>
+      <c r="B7" t="s">
+        <v>32</v>
       </c>
       <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
       <c r="E9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1182,19 +1336,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="3" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1202,164 +1356,152 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
         <v>42</v>
       </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>46</v>
       </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="C10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="E10">
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
         <v>50</v>
       </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
       <c r="E12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1370,4 +1512,112 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" style="3" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="7"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1"/>
+    <hyperlink ref="B11" r:id="rId2"/>
+    <hyperlink ref="B12" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
default values are used for GraphType	Scale	Color	Linewidth	Dash unless the xls spreadsheet provides alternatives.
</commit_message>
<xml_diff>
--- a/plotly-dash/data/pyqt-dash-config.xlsx
+++ b/plotly-dash/data/pyqt-dash-config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22305" windowHeight="11610" tabRatio="686" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22305" windowHeight="11610" tabRatio="686" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="header" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="86">
   <si>
     <t>Dash Experiments</t>
   </si>
@@ -100,9 +100,6 @@
     <t>Z</t>
   </si>
   <si>
-    <t>line</t>
-  </si>
-  <si>
     <t>Rel-speed</t>
   </si>
   <si>
@@ -234,9 +231,6 @@
   </si>
   <si>
     <t>Dash</t>
-  </si>
-  <si>
-    <t>red</t>
   </si>
   <si>
     <t>Linewidth</t>
@@ -701,7 +695,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -715,7 +709,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,30 +729,30 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -766,23 +760,23 @@
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -792,9 +786,6 @@
       <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="3">
-        <v>1</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -806,14 +797,8 @@
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -829,20 +814,14 @@
       <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1</v>
-      </c>
       <c r="F8" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G8" s="3">
         <v>2</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -855,20 +834,14 @@
       <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1</v>
-      </c>
       <c r="F9" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G9" s="3">
         <v>3</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -881,20 +854,14 @@
       <c r="C10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G10" s="3">
         <v>4</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -917,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,30 +902,30 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
         <v>62</v>
-      </c>
-      <c r="G1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
         <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -966,23 +933,23 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -992,25 +959,16 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1021,13 +979,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1035,16 +987,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1052,16 +998,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1082,7 +1022,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D6" sqref="D6:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,30 +1039,30 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
         <v>62</v>
-      </c>
-      <c r="G1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
         <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1130,23 +1070,23 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1156,9 +1096,6 @@
       <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1169,18 +1106,6 @@
       </c>
       <c r="C7" t="s">
         <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1201,7 +1126,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D12"/>
+      <selection activeCell="D5" sqref="D5:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,30 +1143,30 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
         <v>62</v>
-      </c>
-      <c r="G1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1249,23 +1174,23 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1275,50 +1200,38 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1339,7 +1252,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,30 +1269,30 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
         <v>62</v>
-      </c>
-      <c r="G1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1387,23 +1300,23 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1411,10 +1324,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1422,13 +1332,10 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1436,13 +1343,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1450,13 +1354,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1464,10 +1365,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10">
         <v>0.01</v>
@@ -1478,13 +1379,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1492,13 +1390,10 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1518,7 +1413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -1530,15 +1425,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1546,53 +1441,53 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1600,15 +1495,15 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>